<commit_message>
Updates for Surface area, suggests revsiting mont data
</commit_message>
<xml_diff>
--- a/SurfaceArea_SiteChar.xlsx
+++ b/SurfaceArea_SiteChar.xlsx
@@ -68,7 +68,7 @@
     <t>Sites/area</t>
   </si>
   <si>
-    <t>Surface Sites (lit) (mol/g)</t>
+    <t>Surface Sites (lit) (mol)</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,18 +446,18 @@
         <v>0.03</v>
       </c>
       <c r="E2" s="1">
-        <f>C2/D2</f>
+        <f t="shared" ref="E2:E7" si="0">C2/D2</f>
         <v>1.6666666666666668E-3</v>
       </c>
       <c r="F2">
         <v>300</v>
       </c>
       <c r="G2" s="1">
-        <f>E2/F2</f>
+        <f t="shared" ref="G2:G7" si="1">E2/F2</f>
         <v>5.5555555555555558E-6</v>
       </c>
       <c r="H2">
-        <f>30/F2</f>
+        <f t="shared" ref="H2:H7" si="2">30/F2</f>
         <v>0.1</v>
       </c>
       <c r="I2">
@@ -480,22 +480,22 @@
         <v>0.03</v>
       </c>
       <c r="E3" s="1">
-        <f>C3/D3</f>
+        <f t="shared" si="0"/>
         <v>1.75E-3</v>
       </c>
       <c r="F3">
         <v>300</v>
       </c>
       <c r="G3" s="1">
-        <f>E3/F3</f>
+        <f t="shared" si="1"/>
         <v>5.8333333333333331E-6</v>
       </c>
       <c r="H3">
-        <f>30/F3</f>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I7" si="0">3/F3</f>
+        <f t="shared" ref="I3:I7" si="3">3/F3</f>
         <v>0.01</v>
       </c>
     </row>
@@ -510,22 +510,22 @@
         <v>0.03</v>
       </c>
       <c r="E4" s="1">
-        <f>C4/D4</f>
+        <f t="shared" si="0"/>
         <v>3.6666666666666667E-4</v>
       </c>
       <c r="F4">
         <v>25</v>
       </c>
       <c r="G4" s="1">
-        <f>E4/F4</f>
+        <f t="shared" si="1"/>
         <v>1.4666666666666666E-5</v>
       </c>
       <c r="H4">
-        <f>30/F4</f>
+        <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
     </row>
@@ -544,22 +544,22 @@
         <v>0.03</v>
       </c>
       <c r="E5" s="1">
-        <f>C5/D5</f>
+        <f t="shared" si="0"/>
         <v>6.666666666666667E-5</v>
       </c>
       <c r="F5">
         <v>25</v>
       </c>
       <c r="G5" s="1">
-        <f>E5/F5</f>
+        <f t="shared" si="1"/>
         <v>2.6666666666666668E-6</v>
       </c>
       <c r="H5">
-        <f>30/F5</f>
+        <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
     </row>
@@ -578,22 +578,22 @@
         <v>0.04</v>
       </c>
       <c r="E6" s="1">
-        <f>C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2.23E-5</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" s="1">
-        <f>E6/F6</f>
+        <f t="shared" si="1"/>
         <v>2.23E-5</v>
       </c>
       <c r="H6">
-        <f>30/F6</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -612,22 +612,22 @@
         <v>0.03</v>
       </c>
       <c r="E7" s="1">
-        <f>C7/D7</f>
+        <f t="shared" si="0"/>
         <v>6.6666666666666666E-6</v>
       </c>
       <c r="F7">
         <v>80</v>
       </c>
       <c r="G7" s="1">
-        <f>E7/F7</f>
+        <f t="shared" si="1"/>
         <v>8.3333333333333338E-8</v>
       </c>
       <c r="H7">
-        <f>30/F7</f>
+        <f t="shared" si="2"/>
         <v>0.375</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.7499999999999999E-2</v>
       </c>
     </row>

</xml_diff>